<commit_message>
ENH: Update savings example 4
</commit_message>
<xml_diff>
--- a/lifelib/libraries/savings/CashValue_ME_EX4/model_point_moneyness.xlsx
+++ b/lifelib/libraries/savings/CashValue_ME_EX4/model_point_moneyness.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -535,7 +535,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -574,7 +574,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -613,7 +613,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -691,7 +691,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -730,7 +730,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -769,7 +769,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="C9" t="n">

</xml_diff>